<commit_message>
Updated file names and completed preliminary BOM for each board
</commit_message>
<xml_diff>
--- a/Hardware/Bottom/Gamma-BOTTOM-BOM.xlsx
+++ b/Hardware/Bottom/Gamma-BOTTOM-BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orlandohoilett/Documents/Milestones/KickJr/Hardware/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Purdue Milestones\Smartwatch 1\Gamma-Smartwatch\Hardware\Bottom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3201FA0-ADCE-B048-B7EC-E844C06ED99E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97895912-CDC3-4B9A-B49E-D220C3EF4176}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="25580" windowHeight="14540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -225,211 +225,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{4414EC97-401B-5C4D-BF38-03085F1F044A}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Orlando Hoilett:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This is just an example to show you what information to list and how to list them.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{42ADFC76-2A16-3F4B-9937-20E1DF8DC9D9}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Orlando Hoilett:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This is just an example to show you what information to list and how to list them.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{92578C3E-17AC-CF40-B33B-C67DBD723ACA}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Orlando Hoilett:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This is just an example to show you what information to list and how to list them.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{B87F5F84-059E-824D-B1C3-C6D21A6C0FC3}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Orlando Hoilett:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This is just an example to show you what information to list and how to list them.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{8D3ED184-945A-F444-9885-2E4FC0FBB6A7}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Orlando Hoilett:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This is just an example to show you what information to list and how to list them.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{7F187FCD-1E21-9644-AE5D-0FA5E52F65FA}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Orlando Hoilett:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This is just an example to show you what information to list and how to list them.</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>BOM #</t>
   </si>
@@ -458,151 +259,157 @@
     <t>Supplier Part Number</t>
   </si>
   <si>
-    <t>Digi-Key</t>
-  </si>
-  <si>
     <t>Mounting Type</t>
   </si>
   <si>
     <t>Package</t>
   </si>
   <si>
-    <t>SMD</t>
-  </si>
-  <si>
-    <t>Texas Instruments</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
     <t>Price per unit</t>
   </si>
   <si>
-    <t>10k resistor</t>
-  </si>
-  <si>
-    <t>0603</t>
-  </si>
-  <si>
-    <t>Samsung Electro-Mechanics</t>
-  </si>
-  <si>
-    <t>Stackpole Electronics Inc</t>
-  </si>
-  <si>
-    <t>1uF capacitor</t>
-  </si>
-  <si>
-    <t>LM358</t>
-  </si>
-  <si>
-    <t>Photoresistor</t>
-  </si>
-  <si>
-    <t>9V Battery Connector</t>
-  </si>
-  <si>
-    <t>1µF ±10% 25V Ceramic Capacitor X5R 0603 (1608 Metric)</t>
-  </si>
-  <si>
-    <t>CL10A105KA8NNNC</t>
-  </si>
-  <si>
-    <t>1276-1102-1-ND</t>
-  </si>
-  <si>
     <t>Per 100</t>
   </si>
   <si>
-    <t>White  LED Indication - Discrete 2.9V Radial</t>
-  </si>
-  <si>
-    <t>THT</t>
-  </si>
-  <si>
-    <t>Radial</t>
-  </si>
-  <si>
-    <t>American Bright Optoelectronics Corporation</t>
-  </si>
-  <si>
-    <t>BL-BZX3V4V-1-B02</t>
-  </si>
-  <si>
-    <t>BL-BZX3V4V-1-B02-ND</t>
-  </si>
-  <si>
-    <t>White LED</t>
-  </si>
-  <si>
-    <t>Battery Connector, Snap 9V 1 Cell Wire Leads - 4" (101.6mm)</t>
-  </si>
-  <si>
-    <t>Keystone Electronics</t>
-  </si>
-  <si>
-    <t>81-4</t>
-  </si>
-  <si>
-    <t>36-81-4-ND</t>
-  </si>
-  <si>
-    <t>9V</t>
-  </si>
-  <si>
-    <t>LED1</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>General Purpose Amplifier 2 Circuit  8-SOIC</t>
-  </si>
-  <si>
-    <t>8-SOIC</t>
-  </si>
-  <si>
-    <t>LM358DR</t>
-  </si>
-  <si>
-    <t>296-1014-1-ND</t>
-  </si>
-  <si>
-    <t>OP1</t>
-  </si>
-  <si>
     <t>Total (in Bulk)</t>
   </si>
   <si>
-    <t>CDS Cell 520nm 27 ~ 60kOhms @ 10 lux</t>
-  </si>
-  <si>
-    <t>Photo</t>
-  </si>
-  <si>
-    <t>Advanced Photonix</t>
-  </si>
-  <si>
-    <t>PDV-P8104</t>
-  </si>
-  <si>
-    <t>PDV-P8104-ND</t>
-  </si>
-  <si>
-    <t>10 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
-  </si>
-  <si>
-    <t>R1,R2,R3</t>
-  </si>
-  <si>
-    <t>RMCF0603FT10K0</t>
-  </si>
-  <si>
-    <t>RMCF0603FT10K0CT-ND</t>
-  </si>
-  <si>
-    <t>Design Name -- Revision Code / Designer</t>
+    <t>J2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN_07-1.27MM </t>
+  </si>
+  <si>
+    <t>LSM6DS3_CAST</t>
+  </si>
+  <si>
+    <t>IMU1</t>
+  </si>
+  <si>
+    <t>100 nF Capacitor</t>
+  </si>
+  <si>
+    <t>1 uF Capacitor</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>CRYSTALECS-.327-12.5-12-C-TR (CRYSTAL) (32.7680kHz)</t>
+  </si>
+  <si>
+    <t>XTAL2</t>
+  </si>
+  <si>
+    <t>PCF8523</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>S9014E-50-ND</t>
+  </si>
+  <si>
+    <t>GRPB501VWVN-RC</t>
+  </si>
+  <si>
+    <t>Sullins Connector Solutions</t>
+  </si>
+  <si>
+    <t>AD5171</t>
+  </si>
+  <si>
+    <t>AD5242</t>
+  </si>
+  <si>
+    <t>AD5172</t>
+  </si>
+  <si>
+    <t>AD5243</t>
+  </si>
+  <si>
+    <t>TIA</t>
+  </si>
+  <si>
+    <t>NPN-Generic</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Resistor (valueless)</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>C1,C2,C10,C17,C18,C22</t>
+  </si>
+  <si>
+    <t>1M Resistor</t>
+  </si>
+  <si>
+    <t>2.2n Capacitor</t>
+  </si>
+  <si>
+    <t>10M Resistor</t>
+  </si>
+  <si>
+    <t>10k Resistor</t>
+  </si>
+  <si>
+    <t>220k resistor</t>
+  </si>
+  <si>
+    <t>Op amp</t>
+  </si>
+  <si>
+    <t>OP3</t>
+  </si>
+  <si>
+    <t>22n capacitor</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>22u capacitor</t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>R17,R18,R24</t>
+  </si>
+  <si>
+    <t>R14,R22</t>
+  </si>
+  <si>
+    <t>C14,C19</t>
+  </si>
+  <si>
+    <t>R20,R23</t>
+  </si>
+  <si>
+    <t>2.2u capacitor</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>R13,R19,R21</t>
+  </si>
+  <si>
+    <t>Gamma Smartwatch Bottom Board -- Revision A / Gautam Fotedar</t>
+  </si>
+  <si>
+    <t>0.05 spaced Header Pins</t>
+  </si>
+  <si>
+    <t>Connector Header Through Hole 50 position 0.050" (1.27mm)</t>
   </si>
 </sst>
 </file>
@@ -613,7 +420,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -684,14 +491,19 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF444444"/>
+      <name val="Segoe UI Historic"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -707,6 +519,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -856,7 +674,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -884,6 +702,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1314,36 +1135,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" style="1"/>
-    <col min="12" max="12" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="14.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.796875" style="1"/>
+    <col min="12" max="12" width="6.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:16" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="15"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -1352,21 +1173,21 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="M1" s="6">
         <f>SUM(M3:M77)</f>
-        <v>2.48</v>
+        <v>0</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="O1" s="6">
         <f>SUM(O3:O77)</f>
-        <v>1.1271</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="2" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1380,10 +1201,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>11</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>4</v>
@@ -1398,318 +1219,1205 @@
         <v>8</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>6</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="2" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f>1</f>
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" s="10">
-        <v>0.38</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="10"/>
       <c r="L3" s="11">
         <v>1</v>
       </c>
       <c r="M3" s="10">
-        <f t="shared" ref="M3:M8" si="0">K3*L3</f>
-        <v>0.38</v>
-      </c>
-      <c r="N3" s="10">
-        <v>0.1391</v>
-      </c>
+        <f t="shared" ref="M3:M23" si="0">K3*L3</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="10"/>
       <c r="O3" s="10">
-        <f t="shared" ref="O3:O7" si="1">L3*N3</f>
-        <v>0.1391</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+        <f t="shared" ref="O3:O23" si="1">L3*N3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="2" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="K4" s="10">
-        <v>0.89</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="10"/>
       <c r="L4" s="11">
         <v>1</v>
       </c>
       <c r="M4" s="10">
         <f t="shared" si="0"/>
-        <v>0.89</v>
-      </c>
-      <c r="N4" s="10">
-        <v>0.46</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N4" s="10"/>
       <c r="O4" s="10">
         <f t="shared" si="1"/>
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="2" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>29</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
       <c r="F5" s="11"/>
-      <c r="G5" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="K5" s="10">
-        <v>0.55000000000000004</v>
-      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="10"/>
       <c r="L5" s="11">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M5" s="10">
         <f t="shared" si="0"/>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="N5" s="10">
-        <v>0.3982</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N5" s="10"/>
       <c r="O5" s="10">
         <f t="shared" si="1"/>
-        <v>0.3982</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="2" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="10">
-        <v>0.26</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="10"/>
       <c r="L6" s="11">
         <v>1</v>
       </c>
       <c r="M6" s="10">
         <f t="shared" si="0"/>
-        <v>0.26</v>
-      </c>
-      <c r="N6" s="10">
-        <v>9.0899999999999995E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N6" s="10"/>
       <c r="O6" s="10">
         <f t="shared" si="1"/>
-        <v>9.0899999999999995E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" s="2" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>5</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="K7" s="10">
-        <v>0.1</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="10"/>
       <c r="L7" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M7" s="10">
         <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="N7" s="10">
-        <v>6.7999999999999996E-3</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N7" s="10"/>
       <c r="O7" s="10">
         <f t="shared" si="1"/>
-        <v>2.0399999999999998E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" s="2" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>6</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="10">
-        <v>0.1</v>
-      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="10"/>
       <c r="L8" s="11">
         <v>1</v>
       </c>
       <c r="M8" s="10">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="N8" s="10">
-        <v>1.8499999999999999E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N8" s="10"/>
       <c r="O8" s="10">
         <f>L8*N8</f>
-        <v>1.8499999999999999E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2">
+        <v>1</v>
+      </c>
+      <c r="M9" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P9" s="2"/>
+    </row>
+    <row r="10" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="11">
+        <v>1</v>
+      </c>
+      <c r="M10" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="2"/>
+      <c r="O10" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P10" s="2"/>
+    </row>
+    <row r="11" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="11">
+        <v>1</v>
+      </c>
+      <c r="M11" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="2"/>
+      <c r="O11" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P11" s="2"/>
+    </row>
+    <row r="12" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="11">
+        <v>1</v>
+      </c>
+      <c r="M12" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="2"/>
+      <c r="O12" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P12" s="2"/>
+    </row>
+    <row r="13" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2">
+        <v>1</v>
+      </c>
+      <c r="M13" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="2"/>
+      <c r="O13" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="2"/>
+    </row>
+    <row r="14" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="11">
+        <v>1</v>
+      </c>
+      <c r="M14" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="2"/>
+      <c r="O14" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="2"/>
+    </row>
+    <row r="15" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="11">
+        <v>2</v>
+      </c>
+      <c r="M15" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="2"/>
+      <c r="O15" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P15" s="2"/>
+    </row>
+    <row r="16" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="11">
+        <v>2</v>
+      </c>
+      <c r="M16" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="2"/>
+      <c r="O16" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P16" s="2"/>
+    </row>
+    <row r="17" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2">
+        <v>2</v>
+      </c>
+      <c r="M17" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="2"/>
+      <c r="O17" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P17" s="2"/>
+    </row>
+    <row r="18" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="11">
+        <v>3</v>
+      </c>
+      <c r="M18" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="2"/>
+      <c r="O18" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P18" s="2"/>
+    </row>
+    <row r="19" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="11">
+        <v>3</v>
+      </c>
+      <c r="M19" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="2"/>
+      <c r="O19" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P19" s="2"/>
+    </row>
+    <row r="20" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="11">
+        <v>1</v>
+      </c>
+      <c r="M20" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="2"/>
+      <c r="O20" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P20" s="2"/>
+    </row>
+    <row r="21" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="11">
+        <v>1</v>
+      </c>
+      <c r="M21" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="2"/>
+      <c r="O21" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P21" s="2"/>
+    </row>
+    <row r="22" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="11">
+        <v>1</v>
+      </c>
+      <c r="M22" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="2"/>
+      <c r="O22" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P22" s="2"/>
+    </row>
+    <row r="23" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2">
+        <v>1</v>
+      </c>
+      <c r="M23" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N23" s="2"/>
+      <c r="O23" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P23" s="2"/>
+    </row>
+    <row r="24" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+    </row>
+    <row r="25" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+    </row>
+    <row r="26" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+    </row>
+    <row r="27" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+    </row>
+    <row r="28" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+    </row>
+    <row r="29" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+    </row>
+    <row r="30" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+    </row>
+    <row r="31" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+    </row>
+    <row r="32" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+    </row>
+    <row r="33" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+    </row>
+    <row r="34" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+    </row>
+    <row r="35" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+    </row>
+    <row r="36" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+    </row>
+    <row r="37" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+    </row>
+    <row r="38" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+    </row>
+    <row r="39" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+    </row>
+    <row r="40" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+    </row>
+    <row r="41" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+    </row>
+    <row r="42" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+    </row>
+    <row r="43" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+    </row>
+    <row r="44" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+    </row>
+    <row r="45" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+    </row>
+    <row r="46" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+    </row>
+    <row r="47" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+    </row>
+    <row r="48" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+    </row>
+    <row r="49" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+    </row>
+    <row r="50" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+    </row>
+    <row r="51" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>